<commit_message>
Implemented portal pickup, tuned difficulty
</commit_message>
<xml_diff>
--- a/Game testing.xlsx
+++ b/Game testing.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming\Unity\ExpandYourself.git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E2944F-54D2-4B39-9734-514F0759EEBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE32D6DD-0FAF-4A02-B871-2F952596D8ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{84D26F05-005F-4C47-B86A-E61F5CF0D5A3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="38">
   <si>
     <t>Constants:</t>
   </si>
@@ -132,13 +132,28 @@
   </si>
   <si>
     <t>decreased</t>
+  </si>
+  <si>
+    <t>Playtest 3</t>
+  </si>
+  <si>
+    <t>stayed</t>
+  </si>
+  <si>
+    <t>player shrinks too fast on high multipliers</t>
+  </si>
+  <si>
+    <t>Playtest 4</t>
+  </si>
+  <si>
+    <t>Playtest 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -180,8 +195,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,6 +244,11 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -246,7 +274,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -254,8 +282,9 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -266,12 +295,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -280,15 +303,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -299,12 +313,35 @@
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="20% — акцент1" xfId="2" builtinId="30"/>
     <cellStyle name="20% — акцент2" xfId="3" builtinId="34"/>
     <cellStyle name="20% — акцент6" xfId="4" builtinId="50"/>
     <cellStyle name="Контрольная ячейка" xfId="1" builtinId="23"/>
+    <cellStyle name="Нейтральный" xfId="7" builtinId="28"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Плохой" xfId="6" builtinId="27"/>
     <cellStyle name="Хороший" xfId="5" builtinId="26"/>
@@ -619,29 +656,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80A6993C-AE0E-4116-887F-477A7FF7E4AD}">
-  <dimension ref="B1:H74"/>
+  <dimension ref="B1:H185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="H42" sqref="H42"/>
+    <sheetView tabSelected="1" topLeftCell="A161" workbookViewId="0">
+      <selection activeCell="C175" sqref="C175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.796875" style="2"/>
     <col min="2" max="2" width="19.296875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.59765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.59765625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.8984375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.69921875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.796875" style="5"/>
-    <col min="7" max="16384" width="8.796875" style="2"/>
+    <col min="6" max="16384" width="8.796875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" s="1" customFormat="1" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="4"/>
-      <c r="F1" s="4"/>
     </row>
     <row r="2" spans="2:7" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
@@ -655,7 +689,7 @@
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -663,7 +697,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D4" s="2">
@@ -671,7 +705,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D5" s="2">
@@ -679,7 +713,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="2">
@@ -687,7 +721,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="2">
@@ -695,7 +729,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="2">
@@ -703,7 +737,7 @@
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D9" s="2">
@@ -711,7 +745,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="2">
@@ -719,7 +753,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D11" s="2">
@@ -894,17 +928,17 @@
       <c r="B23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -929,7 +963,7 @@
       <c r="B27" s="2">
         <v>1</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="4">
         <v>379</v>
       </c>
       <c r="D27" s="2">
@@ -938,7 +972,7 @@
       <c r="E27" s="2">
         <v>0</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -946,7 +980,7 @@
       <c r="B28" s="2">
         <v>2</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="5">
         <v>289</v>
       </c>
       <c r="D28" s="2">
@@ -960,7 +994,7 @@
       <c r="B29" s="2">
         <v>3</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="5">
         <v>233</v>
       </c>
       <c r="D29" s="2">
@@ -974,7 +1008,7 @@
       <c r="B30" s="2">
         <v>4</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="4">
         <v>332</v>
       </c>
       <c r="D30" s="2">
@@ -988,7 +1022,7 @@
       <c r="B31" s="2">
         <v>5</v>
       </c>
-      <c r="C31" s="8">
+      <c r="C31" s="6">
         <v>172</v>
       </c>
       <c r="D31" s="2">
@@ -1002,7 +1036,7 @@
       <c r="B32" s="2">
         <v>6</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="4">
         <v>199</v>
       </c>
       <c r="D32" s="2">
@@ -1011,7 +1045,7 @@
       <c r="E32" s="2">
         <v>1</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F32" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1019,7 +1053,7 @@
       <c r="B33" s="2">
         <v>7</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C33" s="5">
         <v>147</v>
       </c>
       <c r="D33" s="2">
@@ -1033,7 +1067,7 @@
       <c r="B34" s="2">
         <v>8</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="4">
         <v>125</v>
       </c>
       <c r="D34" s="2">
@@ -1047,7 +1081,7 @@
       <c r="B35" s="2">
         <v>9</v>
       </c>
-      <c r="C35" s="7">
+      <c r="C35" s="5">
         <v>171</v>
       </c>
       <c r="D35" s="2">
@@ -1061,7 +1095,7 @@
       <c r="B36" s="2">
         <v>10</v>
       </c>
-      <c r="C36" s="8">
+      <c r="C36" s="6">
         <v>379</v>
       </c>
       <c r="D36" s="2">
@@ -1075,11 +1109,11 @@
       <c r="B37" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C37" s="12">
+      <c r="C37" s="7">
         <f>AVERAGE(C27:C36)</f>
         <v>242.6</v>
       </c>
-      <c r="D37" s="12">
+      <c r="D37" s="7">
         <f>AVERAGE(D27:D36)</f>
         <v>7.3</v>
       </c>
@@ -1092,8 +1126,6 @@
       <c r="B38" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="F38" s="4"/>
     </row>
     <row r="39" spans="2:8" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="C39" s="2" t="s">
@@ -1107,57 +1139,57 @@
       <c r="B40" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H40" s="13" t="s">
+      <c r="H40" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D41" s="2">
         <v>0.3</v>
       </c>
-      <c r="E41" s="13"/>
-      <c r="H41" s="14" t="s">
+      <c r="E41" s="8"/>
+      <c r="H41" s="9" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="42" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D42" s="2">
         <v>0.06</v>
       </c>
-      <c r="E42" s="14"/>
+      <c r="E42" s="9"/>
     </row>
     <row r="43" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D43" s="2">
         <v>1.75</v>
       </c>
-      <c r="E43" s="14"/>
+      <c r="E43" s="9"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D44" s="2">
         <v>0.15</v>
       </c>
-      <c r="E44" s="14"/>
+      <c r="E44" s="9"/>
     </row>
     <row r="45" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D45" s="2">
@@ -1165,7 +1197,7 @@
       </c>
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D46" s="2">
@@ -1173,7 +1205,7 @@
       </c>
     </row>
     <row r="47" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D47" s="2">
@@ -1181,7 +1213,7 @@
       </c>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D48" s="2">
@@ -1328,17 +1360,17 @@
       <c r="B60" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C60" s="9" t="s">
+      <c r="C60" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C61" s="10" t="s">
+      <c r="C61" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="62" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C62" s="11" t="s">
+      <c r="C62" s="6" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1363,7 +1395,7 @@
       <c r="B64" s="2">
         <v>1</v>
       </c>
-      <c r="C64" s="6">
+      <c r="C64" s="4">
         <v>206</v>
       </c>
       <c r="D64" s="2">
@@ -1373,11 +1405,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B65" s="2">
         <v>2</v>
       </c>
-      <c r="C65" s="7">
+      <c r="C65" s="5">
         <v>494</v>
       </c>
       <c r="D65" s="2">
@@ -1387,11 +1419,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B66" s="2">
         <v>3</v>
       </c>
-      <c r="C66" s="6">
+      <c r="C66" s="4">
         <v>441</v>
       </c>
       <c r="D66" s="2">
@@ -1401,11 +1433,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B67" s="2">
         <v>4</v>
       </c>
-      <c r="C67" s="6">
+      <c r="C67" s="4">
         <v>368</v>
       </c>
       <c r="D67" s="2">
@@ -1415,11 +1447,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B68" s="2">
         <v>5</v>
       </c>
-      <c r="C68" s="6">
+      <c r="C68" s="4">
         <v>185</v>
       </c>
       <c r="D68" s="2">
@@ -1429,11 +1461,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B69" s="2">
         <v>6</v>
       </c>
-      <c r="C69" s="8">
+      <c r="C69" s="6">
         <v>245</v>
       </c>
       <c r="D69" s="2">
@@ -1443,11 +1475,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B70" s="2">
         <v>7</v>
       </c>
-      <c r="C70" s="7">
+      <c r="C70" s="5">
         <v>411</v>
       </c>
       <c r="D70" s="2">
@@ -1457,11 +1489,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B71" s="2">
         <v>8</v>
       </c>
-      <c r="C71" s="7">
+      <c r="C71" s="5">
         <v>191</v>
       </c>
       <c r="D71" s="2">
@@ -1471,11 +1503,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B72" s="2">
         <v>9</v>
       </c>
-      <c r="C72" s="7">
+      <c r="C72" s="5">
         <v>143</v>
       </c>
       <c r="D72" s="2">
@@ -1485,11 +1517,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B73" s="2">
         <v>10</v>
       </c>
-      <c r="C73" s="7">
+      <c r="C73" s="5">
         <v>472</v>
       </c>
       <c r="D73" s="2">
@@ -1499,21 +1531,1298 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B74" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C74" s="12">
+      <c r="C74" s="7">
         <f>AVERAGE(C64:C73)</f>
         <v>315.60000000000002</v>
       </c>
-      <c r="D74" s="12">
+      <c r="D74" s="7">
         <f>AVERAGE(D64:D73)</f>
         <v>8.4</v>
       </c>
       <c r="E74" s="2">
         <f>AVERAGE(E64:E73)</f>
         <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="75" spans="2:8" s="1" customFormat="1" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B75" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="76" spans="2:8" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C76" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D76" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B77" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E77" s="10"/>
+      <c r="H77" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="78" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C78" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D78" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E78" s="15"/>
+      <c r="H78" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="79" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C79" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D79" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="E79" s="16"/>
+      <c r="H79" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="80" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C80" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="E80" s="10"/>
+    </row>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C81" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="E81" s="10"/>
+    </row>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C82" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E82" s="10"/>
+    </row>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C83" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D83" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="E83" s="10"/>
+    </row>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C84" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D84" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E84" s="10"/>
+    </row>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="C85" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D85" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="E85" s="10"/>
+    </row>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B87" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B88" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B89" s="2">
+        <v>1</v>
+      </c>
+      <c r="C89" s="2">
+        <f>D78</f>
+        <v>0.2</v>
+      </c>
+      <c r="D89" s="2">
+        <f>D82</f>
+        <v>0.5</v>
+      </c>
+      <c r="E89" s="2">
+        <f>D84</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B90" s="2">
+        <v>2</v>
+      </c>
+      <c r="C90" s="2">
+        <f>C89+0.075</f>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="D90" s="2">
+        <f>D89+0.03</f>
+        <v>0.53</v>
+      </c>
+      <c r="E90" s="2">
+        <f>E89-0.125</f>
+        <v>1.375</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B91" s="2">
+        <v>3</v>
+      </c>
+      <c r="C91" s="2">
+        <f t="shared" ref="C91:C95" si="7">C90+0.075</f>
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="D91" s="2">
+        <f t="shared" ref="D91:D95" si="8">D90+0.03</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E91" s="2">
+        <f t="shared" ref="E91:E95" si="9">E90-0.125</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B92" s="2">
+        <v>4</v>
+      </c>
+      <c r="C92" s="2">
+        <f t="shared" si="7"/>
+        <v>0.42500000000000004</v>
+      </c>
+      <c r="D92" s="2">
+        <f t="shared" si="8"/>
+        <v>0.59000000000000008</v>
+      </c>
+      <c r="E92" s="2">
+        <f t="shared" si="9"/>
+        <v>1.125</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B93" s="2">
+        <v>5</v>
+      </c>
+      <c r="C93" s="2">
+        <f t="shared" si="7"/>
+        <v>0.5</v>
+      </c>
+      <c r="D93" s="2">
+        <f t="shared" si="8"/>
+        <v>0.62000000000000011</v>
+      </c>
+      <c r="E93" s="2">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B94" s="2">
+        <v>6</v>
+      </c>
+      <c r="C94" s="2">
+        <f t="shared" si="7"/>
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="D94" s="2">
+        <f t="shared" si="8"/>
+        <v>0.65000000000000013</v>
+      </c>
+      <c r="E94" s="2">
+        <f t="shared" si="9"/>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B95" s="2">
+        <v>7</v>
+      </c>
+      <c r="C95" s="2">
+        <f t="shared" si="7"/>
+        <v>0.64999999999999991</v>
+      </c>
+      <c r="D95" s="2">
+        <f t="shared" si="8"/>
+        <v>0.68000000000000016</v>
+      </c>
+      <c r="E95" s="2">
+        <f t="shared" si="9"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B97" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C98" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C99" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B100" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D100" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B101" s="2">
+        <v>1</v>
+      </c>
+      <c r="C101" s="11">
+        <v>244</v>
+      </c>
+      <c r="D101" s="2">
+        <v>7</v>
+      </c>
+      <c r="E101" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B102" s="2">
+        <v>2</v>
+      </c>
+      <c r="C102" s="11">
+        <v>248</v>
+      </c>
+      <c r="D102" s="2">
+        <v>6</v>
+      </c>
+      <c r="E102" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B103" s="2">
+        <v>3</v>
+      </c>
+      <c r="C103" s="11">
+        <v>186</v>
+      </c>
+      <c r="D103" s="2">
+        <v>6</v>
+      </c>
+      <c r="E103" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B104" s="2">
+        <v>4</v>
+      </c>
+      <c r="C104" s="11">
+        <v>141</v>
+      </c>
+      <c r="D104" s="2">
+        <v>6</v>
+      </c>
+      <c r="E104" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B105" s="2">
+        <v>5</v>
+      </c>
+      <c r="C105" s="13">
+        <v>85</v>
+      </c>
+      <c r="D105" s="2">
+        <v>3</v>
+      </c>
+      <c r="E105" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B106" s="2">
+        <v>6</v>
+      </c>
+      <c r="C106" s="11">
+        <v>232</v>
+      </c>
+      <c r="D106" s="2">
+        <v>7</v>
+      </c>
+      <c r="E106" s="2">
+        <v>2</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B107" s="2">
+        <v>7</v>
+      </c>
+      <c r="C107" s="11">
+        <v>14</v>
+      </c>
+      <c r="D107" s="2">
+        <v>1</v>
+      </c>
+      <c r="E107" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B108" s="2">
+        <v>8</v>
+      </c>
+      <c r="C108" s="14">
+        <v>125</v>
+      </c>
+      <c r="D108" s="2">
+        <v>5</v>
+      </c>
+      <c r="E108" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B109" s="2">
+        <v>9</v>
+      </c>
+      <c r="C109" s="11">
+        <v>40</v>
+      </c>
+      <c r="D109" s="2">
+        <v>2</v>
+      </c>
+      <c r="E109" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B110" s="2">
+        <v>10</v>
+      </c>
+      <c r="C110" s="14">
+        <v>141</v>
+      </c>
+      <c r="D110" s="2">
+        <v>5</v>
+      </c>
+      <c r="E110" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="111" spans="2:6" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B111" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C111" s="7">
+        <f>AVERAGE(C101:C110)</f>
+        <v>145.6</v>
+      </c>
+      <c r="D111" s="7">
+        <f>AVERAGE(D101:D110)</f>
+        <v>4.8</v>
+      </c>
+      <c r="E111" s="2">
+        <f>AVERAGE(E101:E110)</f>
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="112" spans="2:6" s="1" customFormat="1" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B112" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="113" spans="2:8" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C113" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D113" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="114" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B114" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C114" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E114" s="10"/>
+      <c r="H114" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="115" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C115" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D115" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="E115" s="10"/>
+      <c r="H115" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="116" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C116" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D116" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E116" s="15"/>
+      <c r="H116" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="117" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C117" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D117" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="E117" s="10"/>
+    </row>
+    <row r="118" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C118" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D118" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="E118" s="10"/>
+    </row>
+    <row r="119" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C119" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D119" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E119" s="10"/>
+    </row>
+    <row r="120" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C120" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D120" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="E120" s="10"/>
+    </row>
+    <row r="121" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C121" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D121" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E121" s="10"/>
+    </row>
+    <row r="122" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C122" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D122" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="E122" s="10"/>
+    </row>
+    <row r="124" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B124" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="125" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B125" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D125" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="126" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B126" s="2">
+        <v>1</v>
+      </c>
+      <c r="C126" s="2">
+        <f>D115</f>
+        <v>0.2</v>
+      </c>
+      <c r="D126" s="2">
+        <f>D119</f>
+        <v>0.5</v>
+      </c>
+      <c r="E126" s="2">
+        <f>D121</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="127" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B127" s="2">
+        <v>2</v>
+      </c>
+      <c r="C127" s="2">
+        <f>C126+0.07</f>
+        <v>0.27</v>
+      </c>
+      <c r="D127" s="2">
+        <f>D126+0.03</f>
+        <v>0.53</v>
+      </c>
+      <c r="E127" s="2">
+        <f>E126-0.125</f>
+        <v>1.375</v>
+      </c>
+    </row>
+    <row r="128" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B128" s="2">
+        <v>3</v>
+      </c>
+      <c r="C128" s="2">
+        <f t="shared" ref="C128:C132" si="10">C127+0.07</f>
+        <v>0.34</v>
+      </c>
+      <c r="D128" s="2">
+        <f t="shared" ref="D128:D132" si="11">D127+0.03</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E128" s="2">
+        <f t="shared" ref="E128:E132" si="12">E127-0.125</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="129" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B129" s="2">
+        <v>4</v>
+      </c>
+      <c r="C129" s="2">
+        <f t="shared" si="10"/>
+        <v>0.41000000000000003</v>
+      </c>
+      <c r="D129" s="2">
+        <f t="shared" si="11"/>
+        <v>0.59000000000000008</v>
+      </c>
+      <c r="E129" s="2">
+        <f t="shared" si="12"/>
+        <v>1.125</v>
+      </c>
+    </row>
+    <row r="130" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B130" s="2">
+        <v>5</v>
+      </c>
+      <c r="C130" s="2">
+        <f t="shared" si="10"/>
+        <v>0.48000000000000004</v>
+      </c>
+      <c r="D130" s="2">
+        <f t="shared" si="11"/>
+        <v>0.62000000000000011</v>
+      </c>
+      <c r="E130" s="2">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B131" s="2">
+        <v>6</v>
+      </c>
+      <c r="C131" s="2">
+        <f t="shared" si="10"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="D131" s="2">
+        <f t="shared" si="11"/>
+        <v>0.65000000000000013</v>
+      </c>
+      <c r="E131" s="2">
+        <f t="shared" si="12"/>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="132" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B132" s="2">
+        <v>7</v>
+      </c>
+      <c r="C132" s="2">
+        <f t="shared" si="10"/>
+        <v>0.62000000000000011</v>
+      </c>
+      <c r="D132" s="2">
+        <f t="shared" si="11"/>
+        <v>0.68000000000000016</v>
+      </c>
+      <c r="E132" s="2">
+        <f t="shared" si="12"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="134" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B134" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="135" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C135" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="136" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C136" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="137" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B137" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C137" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D137" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F137" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="138" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B138" s="2">
+        <v>1</v>
+      </c>
+      <c r="C138" s="14">
+        <v>508</v>
+      </c>
+      <c r="D138" s="12">
+        <v>11</v>
+      </c>
+      <c r="E138" s="12">
+        <v>2</v>
+      </c>
+      <c r="F138" s="12"/>
+    </row>
+    <row r="139" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B139" s="2">
+        <v>2</v>
+      </c>
+      <c r="C139" s="14">
+        <v>50</v>
+      </c>
+      <c r="D139" s="12">
+        <v>3</v>
+      </c>
+      <c r="E139" s="12">
+        <v>1</v>
+      </c>
+      <c r="F139" s="12"/>
+    </row>
+    <row r="140" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B140" s="2">
+        <v>3</v>
+      </c>
+      <c r="C140" s="14">
+        <v>111</v>
+      </c>
+      <c r="D140" s="12">
+        <v>5</v>
+      </c>
+      <c r="E140" s="12">
+        <v>2</v>
+      </c>
+      <c r="F140" s="12"/>
+    </row>
+    <row r="141" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B141" s="2">
+        <v>4</v>
+      </c>
+      <c r="C141" s="14">
+        <v>69</v>
+      </c>
+      <c r="D141" s="12">
+        <v>3</v>
+      </c>
+      <c r="E141" s="12">
+        <v>0</v>
+      </c>
+      <c r="F141" s="12"/>
+    </row>
+    <row r="142" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B142" s="2">
+        <v>5</v>
+      </c>
+      <c r="C142" s="11">
+        <v>81</v>
+      </c>
+      <c r="D142" s="12">
+        <v>4</v>
+      </c>
+      <c r="E142" s="12">
+        <v>2</v>
+      </c>
+      <c r="F142" s="12"/>
+    </row>
+    <row r="143" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B143" s="2">
+        <v>6</v>
+      </c>
+      <c r="C143" s="11">
+        <v>936</v>
+      </c>
+      <c r="D143" s="12">
+        <v>15</v>
+      </c>
+      <c r="E143" s="12">
+        <v>2</v>
+      </c>
+      <c r="F143" s="12"/>
+    </row>
+    <row r="144" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B144" s="2">
+        <v>7</v>
+      </c>
+      <c r="C144" s="11">
+        <v>519</v>
+      </c>
+      <c r="D144" s="12">
+        <v>11</v>
+      </c>
+      <c r="E144" s="12">
+        <v>2</v>
+      </c>
+      <c r="F144" s="12"/>
+    </row>
+    <row r="145" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B145" s="2">
+        <v>8</v>
+      </c>
+      <c r="C145" s="11">
+        <v>364</v>
+      </c>
+      <c r="D145" s="12">
+        <v>9</v>
+      </c>
+      <c r="E145" s="12">
+        <v>2</v>
+      </c>
+      <c r="F145" s="12"/>
+    </row>
+    <row r="146" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B146" s="2">
+        <v>9</v>
+      </c>
+      <c r="C146" s="14">
+        <v>991</v>
+      </c>
+      <c r="D146" s="12">
+        <v>14</v>
+      </c>
+      <c r="E146" s="12">
+        <v>1</v>
+      </c>
+      <c r="F146" s="12"/>
+    </row>
+    <row r="147" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B147" s="2">
+        <v>10</v>
+      </c>
+      <c r="C147" s="11">
+        <v>169</v>
+      </c>
+      <c r="D147" s="12">
+        <v>6</v>
+      </c>
+      <c r="E147" s="12">
+        <v>1</v>
+      </c>
+      <c r="F147" s="12"/>
+    </row>
+    <row r="148" spans="2:8" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B148" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C148" s="7">
+        <f>AVERAGE(C138:C147)</f>
+        <v>379.8</v>
+      </c>
+      <c r="D148" s="7">
+        <f>AVERAGE(D138:D147)</f>
+        <v>8.1</v>
+      </c>
+      <c r="E148" s="2">
+        <f>AVERAGE(E138:E147)</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="149" spans="2:8" s="1" customFormat="1" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B149" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="150" spans="2:8" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="C150" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="151" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B151" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E151" s="10"/>
+      <c r="H151" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="152" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C152" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D152" s="2">
+        <v>0.21</v>
+      </c>
+      <c r="E152" s="8"/>
+      <c r="H152" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="153" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C153" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D153" s="2">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="E153" s="16"/>
+      <c r="H153" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="154" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C154" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D154" s="2">
+        <v>1.75</v>
+      </c>
+      <c r="E154" s="10"/>
+    </row>
+    <row r="155" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C155" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D155" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="E155" s="10"/>
+    </row>
+    <row r="156" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C156" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D156" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E156" s="10"/>
+    </row>
+    <row r="157" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C157" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D157" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="E157" s="10"/>
+    </row>
+    <row r="158" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C158" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D158" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E158" s="10"/>
+    </row>
+    <row r="159" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="C159" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D159" s="2">
+        <v>0.125</v>
+      </c>
+      <c r="E159" s="10"/>
+    </row>
+    <row r="161" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B161" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="162" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B162" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D162" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E162" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="163" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B163" s="2">
+        <v>1</v>
+      </c>
+      <c r="C163" s="2">
+        <f>D152</f>
+        <v>0.21</v>
+      </c>
+      <c r="D163" s="2">
+        <f>D156</f>
+        <v>0.5</v>
+      </c>
+      <c r="E163" s="2">
+        <f>D158</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="164" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B164" s="2">
+        <v>2</v>
+      </c>
+      <c r="C164" s="2">
+        <f>C163+0.0725</f>
+        <v>0.28249999999999997</v>
+      </c>
+      <c r="D164" s="2">
+        <f>D163+0.03</f>
+        <v>0.53</v>
+      </c>
+      <c r="E164" s="2">
+        <f>E163-0.125</f>
+        <v>1.375</v>
+      </c>
+    </row>
+    <row r="165" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B165" s="2">
+        <v>3</v>
+      </c>
+      <c r="C165" s="2">
+        <f t="shared" ref="C165:C169" si="13">C164+0.0725</f>
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="D165" s="2">
+        <f t="shared" ref="D165:D169" si="14">D164+0.03</f>
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E165" s="2">
+        <f t="shared" ref="E165:E169" si="15">E164-0.125</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="166" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B166" s="2">
+        <v>4</v>
+      </c>
+      <c r="C166" s="2">
+        <f t="shared" si="13"/>
+        <v>0.42749999999999999</v>
+      </c>
+      <c r="D166" s="2">
+        <f t="shared" si="14"/>
+        <v>0.59000000000000008</v>
+      </c>
+      <c r="E166" s="2">
+        <f t="shared" si="15"/>
+        <v>1.125</v>
+      </c>
+    </row>
+    <row r="167" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B167" s="2">
+        <v>5</v>
+      </c>
+      <c r="C167" s="2">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="D167" s="2">
+        <f t="shared" si="14"/>
+        <v>0.62000000000000011</v>
+      </c>
+      <c r="E167" s="2">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B168" s="2">
+        <v>6</v>
+      </c>
+      <c r="C168" s="2">
+        <f t="shared" si="13"/>
+        <v>0.57250000000000001</v>
+      </c>
+      <c r="D168" s="2">
+        <f t="shared" si="14"/>
+        <v>0.65000000000000013</v>
+      </c>
+      <c r="E168" s="2">
+        <f t="shared" si="15"/>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="169" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B169" s="2">
+        <v>7</v>
+      </c>
+      <c r="C169" s="2">
+        <f t="shared" si="13"/>
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="D169" s="2">
+        <f t="shared" si="14"/>
+        <v>0.68000000000000016</v>
+      </c>
+      <c r="E169" s="2">
+        <f t="shared" si="15"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="171" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B171" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C171" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="172" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C172" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="173" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C173" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="174" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B174" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C174" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D174" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E174" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F174" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="175" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B175" s="2">
+        <v>1</v>
+      </c>
+      <c r="C175" s="17">
+        <v>114</v>
+      </c>
+      <c r="D175">
+        <v>5</v>
+      </c>
+      <c r="E175">
+        <v>1</v>
+      </c>
+      <c r="F175" s="12"/>
+    </row>
+    <row r="176" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B176" s="2">
+        <v>2</v>
+      </c>
+      <c r="C176"/>
+      <c r="D176"/>
+      <c r="E176"/>
+      <c r="F176" s="12"/>
+    </row>
+    <row r="177" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B177" s="2">
+        <v>3</v>
+      </c>
+      <c r="C177"/>
+      <c r="D177"/>
+      <c r="E177"/>
+      <c r="F177" s="12"/>
+    </row>
+    <row r="178" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B178" s="2">
+        <v>4</v>
+      </c>
+      <c r="C178"/>
+      <c r="D178"/>
+      <c r="E178"/>
+      <c r="F178" s="12"/>
+    </row>
+    <row r="179" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B179" s="2">
+        <v>5</v>
+      </c>
+      <c r="C179"/>
+      <c r="D179"/>
+      <c r="E179"/>
+      <c r="F179" s="12"/>
+    </row>
+    <row r="180" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B180" s="2">
+        <v>6</v>
+      </c>
+      <c r="C180"/>
+      <c r="D180"/>
+      <c r="E180"/>
+      <c r="F180" s="12"/>
+    </row>
+    <row r="181" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B181" s="2">
+        <v>7</v>
+      </c>
+      <c r="C181"/>
+      <c r="D181"/>
+      <c r="E181"/>
+      <c r="F181" s="12"/>
+    </row>
+    <row r="182" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B182" s="2">
+        <v>8</v>
+      </c>
+      <c r="C182"/>
+      <c r="D182"/>
+      <c r="E182"/>
+      <c r="F182" s="12"/>
+    </row>
+    <row r="183" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B183" s="2">
+        <v>9</v>
+      </c>
+      <c r="C183"/>
+      <c r="D183"/>
+      <c r="E183"/>
+      <c r="F183" s="12"/>
+    </row>
+    <row r="184" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B184" s="2">
+        <v>10</v>
+      </c>
+      <c r="C184"/>
+      <c r="D184"/>
+      <c r="E184"/>
+      <c r="F184" s="12"/>
+    </row>
+    <row r="185" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B185" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C185" s="7">
+        <f>AVERAGE(C175:C184)</f>
+        <v>114</v>
+      </c>
+      <c r="D185" s="7">
+        <f>AVERAGE(D175:D184)</f>
+        <v>5</v>
+      </c>
+      <c r="E185" s="2">
+        <f>AVERAGE(E175:E184)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>